<commit_message>
changed the location of sim score of trial 3 and generated their visuals
</commit_message>
<xml_diff>
--- a/RESULTS/stats_comments.xlsx
+++ b/RESULTS/stats_comments.xlsx
@@ -470,47 +470,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_1_temps_1.3_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_1_temps_1.3_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_0_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_0_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-4-turbo-preview_n_5_tempr_0_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-4-turbo-preview_n_5_tempr_0_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_1_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_15_tempr_1_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_0_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_0_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_10_tempr_0_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_10_tempr_0_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_3_tempr_0_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_3_tempr_0_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_1_temps_1_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_1_temps_1_trial_3_sim_score.csv</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>./RESULTS/final scores/trial 3/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_0_temps_1.5_trial_3_sim_score.csv</t>
+          <t>./RESULTS/trial 3/trial 3 results/dataset_HumanEval_model_gpt-3.5-turbo_n_5_tempr_0_temps_1.5_trial_3_sim_score.csv</t>
         </is>
       </c>
     </row>

</xml_diff>